<commit_message>
Acer950 major on noNeedUSA
</commit_message>
<xml_diff>
--- a/msff/xls/noNeedUSA.xlsx
+++ b/msff/xls/noNeedUSA.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A940DDE-85DD-4727-B52F-884AC8B5B3F1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C735C948-EC2A-494F-B0E5-22B16CCF4F4A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1230" yWindow="2355" windowWidth="14415" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="numbers extracted" sheetId="2" r:id="rId2"/>
+    <sheet name="MSExcel tricks" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>cpf</t>
   </si>
@@ -44,12 +44,6 @@
     <t>dry-up[2]</t>
   </si>
   <si>
-    <t>incr to 4k/M</t>
-  </si>
-  <si>
-    <t>non-CPF[1]</t>
-  </si>
-  <si>
     <t>tgt bal</t>
   </si>
   <si>
@@ -57,9 +51,6 @@
   </si>
   <si>
     <t>4.5Y window</t>
-  </si>
-  <si>
-    <t>cpfLife/M assum` $3000</t>
   </si>
   <si>
     <t xml:space="preserve">ZLH age:
@@ -70,9 +61,6 @@
 Jan-74</t>
   </si>
   <si>
-    <t>burnrate/M assum` $6000</t>
-  </si>
-  <si>
     <t>&lt;- At this juncture, both kids edu done. Burn rate=&gt;3k/M</t>
   </si>
   <si>
@@ -80,10 +68,6 @@
 TopUp</t>
   </si>
   <si>
-    <t>sal/Y assum`
-$150,000</t>
-  </si>
-  <si>
     <t>&lt;-top up to wife cprRA[3]</t>
   </si>
   <si>
@@ -97,30 +81,53 @@
   </si>
   <si>
     <t>[4] 200k sounds like decent reserve, but there is no minimum IMO</t>
+  </si>
+  <si>
+    <t>cpfLife/M $3000</t>
+  </si>
+  <si>
+    <t>4k/M?</t>
+  </si>
+  <si>
+    <t>non-CPF
+[1]</t>
+  </si>
+  <si>
+    <t>sal/Y
+$100,000</t>
+  </si>
+  <si>
+    <t>burnRate/M $6000</t>
+  </si>
+  <si>
+    <t>dateval</t>
+  </si>
+  <si>
+    <t>extractor formula</t>
+  </si>
+  <si>
+    <t>prefix "age" or suffix "k"</t>
+  </si>
+  <si>
+    <t>dateDif</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="6">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
     <numFmt numFmtId="166" formatCode="mmm/yyyy"/>
+    <numFmt numFmtId="167" formatCode="&quot;age&quot;\ 00.0"/>
+    <numFmt numFmtId="168" formatCode="General&quot;k&quot;"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -134,6 +141,20 @@
     <font>
       <sz val="8"/>
       <color theme="0" tint="-0.14999847407452621"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -202,40 +223,45 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="17" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="6" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="17" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -519,350 +545,350 @@
   <dimension ref="B2:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.5703125" customWidth="1"/>
     <col min="2" max="2" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="1.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="7"/>
-    <col min="12" max="12" width="9.140625" style="14"/>
+    <col min="5" max="5" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="2"/>
+    <col min="12" max="12" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="15"/>
-      <c r="E2" s="22">
+      <c r="B2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="E2" s="6">
         <f>DATEVALUE(CLEAN(RIGHT(E3,LEN(E3)-FIND(":",E3))))</f>
         <v>28672</v>
       </c>
-      <c r="F2" s="22">
+      <c r="F2" s="6">
         <f>DATEVALUE(CLEAN(RIGHT(F3,LEN(F3)-FIND(":",F3))))</f>
         <v>27030</v>
       </c>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23" t="str">
+      <c r="G2" s="7"/>
+      <c r="H2" s="7" t="str">
         <f>RIGHT(H3,LEN(H3)-FIND("$",H3))</f>
         <v>6000</v>
       </c>
-      <c r="I2" s="23" t="str">
+      <c r="I2" s="7" t="str">
         <f>RIGHT(I3,LEN(I3)-FIND("$",I3))</f>
-        <v>150,000</v>
-      </c>
-      <c r="J2" s="23" t="str">
+        <v>100,000</v>
+      </c>
+      <c r="J2" s="7" t="str">
         <f>RIGHT(I13,LEN(I13)-FIND("$",I13))</f>
         <v>3000</v>
       </c>
     </row>
-    <row r="3" spans="2:12" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
+    <row r="3" spans="2:12" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B3" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="18" t="s">
+      <c r="C3" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="20"/>
+      <c r="E3" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="16"/>
-      <c r="L3" s="14"/>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="3"/>
-      <c r="C4" s="3">
-        <v>770</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="5">
-        <f>YEARFRAC($E$2,G4)</f>
-        <v>43.416666666666664</v>
-      </c>
-      <c r="F4" s="4">
-        <f>YEARFRAC($F$2,G4)</f>
-        <v>47.916666666666664</v>
-      </c>
-      <c r="G4" s="6">
+      <c r="K3" s="4"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="10"/>
+      <c r="C4" s="27">
+        <v>1120</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="26">
+        <f>DATEDIF($E$2,G4,"y")</f>
+        <v>43</v>
+      </c>
+      <c r="F4" s="26">
+        <f>DATEDIF($F$2,G4,"y")</f>
+        <v>47</v>
+      </c>
+      <c r="G4" s="12">
         <v>44531</v>
       </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="6" t="s">
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+    </row>
+    <row r="5" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="27">
         <f>-DATEDIF(G4,G8, "m")*$H$2/1000</f>
         <v>-504</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="27">
         <f>DATEDIF(G4,G8, "y")*$I$2/1000</f>
-        <v>1050</v>
-      </c>
-      <c r="J5" s="3"/>
-      <c r="L5" s="14" t="str">
+        <v>700</v>
+      </c>
+      <c r="J5" s="10"/>
+      <c r="L5" s="3" t="str">
         <f ca="1">IFERROR(MID(#REF!,ROW(INDIRECT("1:"&amp;LEN(#REF!))),1)*1,"")</f>
         <v/>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="5">
-        <f>YEARFRAC($E$2,G6)</f>
-        <v>50.416666666666664</v>
-      </c>
-      <c r="F6" s="4">
-        <f>YEARFRAC($F$2,G6)</f>
-        <v>54.916666666666664</v>
-      </c>
-      <c r="G6" s="6">
+    <row r="6" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="26">
+        <f>DATEDIF($E$2,G6,"y")</f>
+        <v>50</v>
+      </c>
+      <c r="F6" s="26">
+        <f>DATEDIF($F$2,G6,"y")</f>
+        <v>54</v>
+      </c>
+      <c r="G6" s="12">
         <v>47088</v>
       </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3" t="s">
+      <c r="H6" s="10"/>
+      <c r="I6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="3"/>
-      <c r="L6" s="14" t="str">
+      <c r="J6" s="10"/>
+      <c r="L6" s="3" t="str">
         <f ca="1">_xlfn.TEXTJOIN("",TRUE,L5)</f>
         <v/>
       </c>
     </row>
     <row r="7" spans="2:12" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
-      <c r="C8" s="3">
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+    </row>
+    <row r="8" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="10"/>
+      <c r="C8" s="27">
         <f>C4+SUM(H5:J5)</f>
         <v>1316</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="5">
-        <f>YEARFRAC($E$2,G8)</f>
-        <v>50.416666666666664</v>
-      </c>
-      <c r="F8" s="4">
-        <f>YEARFRAC($F$2,G8)</f>
-        <v>54.916666666666664</v>
-      </c>
-      <c r="G8" s="6">
+      <c r="D8" s="10"/>
+      <c r="E8" s="26">
+        <f>DATEDIF($E$2,G8,"y")</f>
+        <v>50</v>
+      </c>
+      <c r="F8" s="26">
+        <f>DATEDIF($F$2,G8,"y")</f>
+        <v>54</v>
+      </c>
+      <c r="G8" s="12">
         <v>47088</v>
       </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="J8" s="2"/>
-      <c r="L8" s="14" t="str">
+      <c r="H8" s="10"/>
+      <c r="I8" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="13"/>
+      <c r="L8" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(L5)</f>
         <v/>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="6" t="s">
+    <row r="9" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="27">
         <f>-DATEDIF(G8,G10, "m")*$H$2/1000</f>
         <v>-504</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="27">
         <v>-400</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="27">
         <v>-200</v>
       </c>
-      <c r="K9" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-      <c r="C10" s="3">
+      <c r="K9" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="10"/>
+      <c r="C10" s="27">
         <f>C8+SUM(H9:J9)</f>
         <v>212</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="5">
-        <f>YEARFRAC($E$2,G10)</f>
-        <v>57.416666666666664</v>
-      </c>
-      <c r="F10" s="4">
-        <f>YEARFRAC($F$2,G10)</f>
-        <v>61.916666666666664</v>
-      </c>
-      <c r="G10" s="6">
+      <c r="D10" s="10"/>
+      <c r="E10" s="26">
+        <f>DATEDIF($E$2,G10,"y")</f>
+        <v>57</v>
+      </c>
+      <c r="F10" s="26">
+        <f>DATEDIF($F$2,G10,"y")</f>
+        <v>61</v>
+      </c>
+      <c r="G10" s="12">
         <v>49644</v>
       </c>
-      <c r="H10" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="2"/>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="6" t="s">
+      <c r="H10" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="13"/>
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="27">
         <f>-DATEDIF(G10,G13, "m")*3</f>
         <v>-111</v>
       </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3">
+      <c r="I11" s="10"/>
+      <c r="J11" s="27">
         <v>-100</v>
       </c>
-      <c r="K11" s="7" t="s">
-        <v>19</v>
+      <c r="K11" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="2:12" ht="1.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-    </row>
-    <row r="13" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
-      <c r="C13" s="3">
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+    </row>
+    <row r="13" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B13" s="10"/>
+      <c r="C13" s="10">
         <f>C10+SUM(H11:J11)</f>
         <v>1</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="4">
-        <f>YEARFRAC($F$2,G13)</f>
+      <c r="D13" s="10"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="26">
+        <f>DATEDIF($F$2,G13,"y")</f>
         <v>65</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="12">
         <v>50771</v>
       </c>
-      <c r="H13" s="3"/>
-      <c r="I13" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="J13" s="3"/>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H14" s="3">
+      <c r="H13" s="10"/>
+      <c r="I13" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" s="10"/>
+    </row>
+    <row r="14" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="27">
         <f>-DATEDIF(G13,G15, "m")*3</f>
         <v>-162</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14" s="27">
         <f>DATEDIF(G13,G15, "m")*J2/1000</f>
         <v>162</v>
       </c>
-      <c r="J14" s="3"/>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="3"/>
-      <c r="C15" s="3">
+      <c r="J14" s="10"/>
+    </row>
+    <row r="15" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="10"/>
+      <c r="C15" s="10">
         <f>C13+SUM(H14:J14)</f>
         <v>1</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="5">
-        <f>YEARFRAC($E$2,G15)</f>
+      <c r="D15" s="10"/>
+      <c r="E15" s="26">
+        <f>DATEDIF($E$2,G15,"y")</f>
         <v>65</v>
       </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="6">
+      <c r="F15" s="13"/>
+      <c r="G15" s="12">
         <v>52413</v>
       </c>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J15" s="3"/>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J15" s="10"/>
+    </row>
+    <row r="16" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+    </row>
+    <row r="17" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
@@ -882,17 +908,17 @@
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="24" t="s">
-        <v>20</v>
+      <c r="B22" s="8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="24" t="s">
-        <v>23</v>
+      <c r="B23" s="8" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -906,14 +932,38 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{658ED645-D1CA-42ED-8997-C95A14CF61B9}">
-  <dimension ref="A1"/>
+  <dimension ref="B3:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="43.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>